<commit_message>
code clean and generic
</commit_message>
<xml_diff>
--- a/src/main/resources/Scheduler.xlsx
+++ b/src/main/resources/Scheduler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\barco\process\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\100K\process\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73CDB800-41BC-40A2-9F4F-09F44CB81258}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9778F3B9-05BB-4ADD-9854-C2E275A3C67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3A3082B2-3BF6-48FE-9E5C-DA2588D0FD1A}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Job Name</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31</t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>14</v>
@@ -692,7 +695,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
new filed added into xlsx for task and job
</commit_message>
<xml_diff>
--- a/src/main/resources/Scheduler.xlsx
+++ b/src/main/resources/Scheduler.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Job Name</t>
   </si>
@@ -38,6 +38,18 @@
     <t>Recurrence</t>
   </si>
   <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Email Job Complete</t>
+  </si>
+  <si>
+    <t>Email Job Fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email Job Skip </t>
+  </si>
+  <si>
     <t>Filed Name</t>
   </si>
   <si>
@@ -75,6 +87,21 @@
   </si>
   <si>
     <t>Recurrence Add the mint or hr for mint(1-59) or for hr(1-12) or weekly (Sunday-Monday) or monthly (1-31) any 1 day</t>
+  </si>
+  <si>
+    <t>Thread Priority</t>
+  </si>
+  <si>
+    <t>Email job complete</t>
+  </si>
+  <si>
+    <t>Check True|False can be use to  email</t>
+  </si>
+  <si>
+    <t>Email job fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email job skip </t>
   </si>
   <si>
     <t>Note</t>
@@ -112,12 +139,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,13 +162,30 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF202124"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,7 +199,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -170,22 +244,23 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -200,29 +275,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -231,17 +283,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,37 +312,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,109 +340,193 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -417,89 +536,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -520,14 +587,38 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -550,7 +641,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -573,56 +679,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -631,7 +687,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -649,134 +705,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -788,10 +844,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -799,8 +859,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1062,44 +1122,59 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.6363636363636" customWidth="1"/>
-    <col min="2" max="2" width="16.2727272727273" customWidth="1"/>
-    <col min="3" max="3" width="14.6363636363636" customWidth="1"/>
-    <col min="4" max="4" width="16.4545454545455" customWidth="1"/>
-    <col min="5" max="5" width="16.2727272727273" customWidth="1"/>
-    <col min="6" max="6" width="15.7272727272727" customWidth="1"/>
-    <col min="7" max="7" width="15.5454545454545" customWidth="1"/>
+    <col min="1" max="1" width="9.72727272727273" customWidth="1"/>
+    <col min="2" max="2" width="13.1818181818182" customWidth="1"/>
+    <col min="3" max="3" width="10.1818181818182" customWidth="1"/>
+    <col min="4" max="4" width="9.18181818181818" customWidth="1"/>
+    <col min="5" max="6" width="10.2727272727273" customWidth="1"/>
+    <col min="7" max="7" width="11.0909090909091" customWidth="1"/>
+    <col min="8" max="8" width="7.72727272727273" customWidth="1"/>
+    <col min="9" max="9" width="18.5454545454545" customWidth="1"/>
+    <col min="10" max="10" width="12.6363636363636" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1111,10 +1186,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C1000"/>
+  <dimension ref="A1:C1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15" customHeight="1" outlineLevelCol="2"/>
@@ -1127,13 +1202,13 @@
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:3">
@@ -1141,21 +1216,21 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:3">
@@ -1163,10 +1238,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:3">
@@ -1174,10 +1249,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:3">
@@ -1185,10 +1260,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:3">
@@ -1196,10 +1271,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1" spans="1:3">
@@ -1207,67 +1282,107 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" ht="14.25" customHeight="1" spans="1:3">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" ht="14.25" customHeight="1" spans="1:3">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1" spans="2:3">
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>21</v>
+    <row r="11" ht="14.25" customHeight="1" spans="1:3">
+      <c r="A11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1" spans="2:3">
-      <c r="B11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>23</v>
+    <row r="12" ht="14.25" customHeight="1" spans="1:3">
+      <c r="A12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1" spans="2:3">
-      <c r="B12" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" ht="14.25" customHeight="1" spans="2:3">
-      <c r="B13" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" ht="14.25" customHeight="1" spans="2:3">
-      <c r="B14" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
+    <row r="13" ht="14.25" customHeight="1"/>
+    <row r="14" ht="14.25" customHeight="1"/>
     <row r="15" ht="14.25" customHeight="1" spans="2:3">
       <c r="B15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>28</v>
+      <c r="C15" s="8" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="17" ht="14.25" customHeight="1" spans="2:3">
+      <c r="B17" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" customHeight="1" spans="2:3">
+      <c r="B18" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" customHeight="1" spans="2:3">
+      <c r="B19" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" customHeight="1" spans="2:3">
+      <c r="B20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" customHeight="1" spans="2:3">
+      <c r="B21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
     <row r="22" ht="14.25" customHeight="1"/>
     <row r="23" ht="14.25" customHeight="1"/>
     <row r="24" ht="14.25" customHeight="1"/>
@@ -2247,6 +2362,7 @@
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>